<commit_message>
Mise à jour du cours
</commit_message>
<xml_diff>
--- a/classeurs/fonction_nbsi.xlsx
+++ b/classeurs/fonction_nbsi.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Activité 6" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Activité 7" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Activité 5" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Activité 6" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Activité 7" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+  <si>
+    <t xml:space="preserve">Nom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Age</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Majeur/Mineur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kaïs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kamel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kassem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Karem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Majeurs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mineurs</t>
+  </si>
   <si>
     <t xml:space="preserve">Nom &amp; Prénom</t>
   </si>
@@ -93,6 +124,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -110,15 +142,17 @@
       <family val="0"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -197,7 +231,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -206,51 +240,55 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="255" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -331,15 +369,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -349,67 +388,73 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="2" t="n">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="B3" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="B4" s="3" t="n">
+        <v>17</v>
+      </c>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="B5" s="3" t="n">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>21</v>
+      </c>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
       <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="7"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="7"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -422,26 +467,117 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="5"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>14</v>
+      <c r="A1" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -451,7 +587,7 @@
       <c r="B2" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="C2" s="9" t="n">
+      <c r="C2" s="10" t="n">
         <f aca="false">ROUND(B2*A2,0)</f>
         <v>186</v>
       </c>
@@ -467,7 +603,7 @@
       <c r="B3" s="3" t="n">
         <v>5.6</v>
       </c>
-      <c r="C3" s="10" t="n">
+      <c r="C3" s="11" t="n">
         <f aca="false">ROUND(B3*A3,0)</f>
         <v>67</v>
       </c>
@@ -483,7 +619,7 @@
       <c r="B4" s="3" t="n">
         <v>9.8</v>
       </c>
-      <c r="C4" s="10" t="n">
+      <c r="C4" s="11" t="n">
         <f aca="false">ROUND(B4*A4,0)</f>
         <v>31</v>
       </c>
@@ -499,7 +635,7 @@
       <c r="B5" s="3" t="n">
         <v>5.2</v>
       </c>
-      <c r="C5" s="10" t="n">
+      <c r="C5" s="11" t="n">
         <f aca="false">ROUND(B5*A5,0)</f>
         <v>81</v>
       </c>
@@ -515,7 +651,7 @@
       <c r="B6" s="3" t="n">
         <v>9.1</v>
       </c>
-      <c r="C6" s="10" t="n">
+      <c r="C6" s="11" t="n">
         <f aca="false">ROUND(B6*A6,0)</f>
         <v>112</v>
       </c>
@@ -531,7 +667,7 @@
       <c r="B7" s="4" t="n">
         <v>12.5</v>
       </c>
-      <c r="C7" s="11" t="n">
+      <c r="C7" s="12" t="n">
         <f aca="false">ROUND(B7*A7,0)</f>
         <v>105</v>
       </c>
@@ -541,36 +677,36 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="7"/>
+      <c r="A9" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="7"/>
+      <c r="A10" s="13"/>
+      <c r="B10" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="7"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -581,7 +717,7 @@
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Mise à jour des activité et du cours Excel
</commit_message>
<xml_diff>
--- a/classeurs/fonction_nbsi.xlsx
+++ b/classeurs/fonction_nbsi.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Activité 5" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Activité 6" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Activité 7" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Activité 9" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Activité 10" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Activité 11" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -371,11 +371,11 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.43"/>
@@ -456,8 +456,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -473,7 +473,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.71"/>
   </cols>
@@ -547,8 +547,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -560,11 +560,11 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="9" t="s">
@@ -719,8 +719,8 @@
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>